<commit_message>
with wrk, on 4 core cpu
</commit_message>
<xml_diff>
--- a/results/xeon_4_core-max100-localhost.xlsx
+++ b/results/xeon_4_core-max100-localhost.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
-  <workbookPr showInkAnnotation="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fat/worx/tmp/ws-benchmark/results/"/>
@@ -24,28 +24,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>concurrent connections</t>
+    <t>actix-diesel</t>
+  </si>
+  <si>
+    <t>actix-tokio</t>
   </si>
   <si>
     <t>spider-gazelle</t>
   </si>
   <si>
-    <t>actix-diesel</t>
+    <t>X=1</t>
   </si>
   <si>
-    <t>spring</t>
+    <t>X=2</t>
   </si>
   <si>
-    <t>kemal</t>
+    <t>X=4</t>
+  </si>
+  <si>
+    <t>spider-gazelle-mt</t>
+  </si>
+  <si>
+    <t>X=8</t>
+  </si>
+  <si>
+    <t>X=16</t>
+  </si>
+  <si>
+    <t>X=32</t>
+  </si>
+  <si>
+    <t>X=64</t>
+  </si>
+  <si>
+    <t>wrk -t1 -cX -d10s http://…</t>
+  </si>
+  <si>
+    <t>mt: compiled with -Dpreview_mt</t>
+  </si>
+  <si>
+    <t>NOTES :</t>
+  </si>
+  <si>
+    <t>fasthttp-router</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,12 +92,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Courier"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,8 +144,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -104,22 +174,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -167,7 +303,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Localhost Test</a:t>
+              <a:t>Xeon E3-1225 v5  3.30GHz, 4 cores cpu</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -213,11 +349,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>concurrent connections</c:v>
+                  <c:v>actix-diesel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -235,61 +371,60 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$I$3</c:f>
+              <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>X=1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>X=2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>X=4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>X=8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>X=16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>X=32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>X=64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$C$4:$I$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>6570.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>11995.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>19384.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>20083.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>22241.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>23967.68</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.0</c:v>
+                  <c:v>24547.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -301,11 +436,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>spider-gazelle</c:v>
+                  <c:v>actix-tokio</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -323,61 +458,60 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$I$3</c:f>
+              <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>X=1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>X=2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>X=4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>X=8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>X=16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>X=32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>X=64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>Sheet1!$C$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9631.35</c:v>
+                  <c:v>11893.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18261.42</c:v>
+                  <c:v>23415.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25336.34</c:v>
+                  <c:v>30027.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25010.38</c:v>
+                  <c:v>35027.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23253.83</c:v>
+                  <c:v>40493.51</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22220.29</c:v>
+                  <c:v>45090.82</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20957.41</c:v>
+                  <c:v>48192.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,11 +523,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>actix-diesel</c:v>
+                  <c:v>spider-gazelle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -411,61 +545,60 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$I$3</c:f>
+              <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>X=1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>X=2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>X=4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>X=8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>X=16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>X=32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>X=64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$9</c:f>
+              <c:f>Sheet1!$C$6:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6324.46</c:v>
+                  <c:v>11152.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11880.28</c:v>
+                  <c:v>19495.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17684.82</c:v>
+                  <c:v>31390.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20198.53</c:v>
+                  <c:v>29760.47</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21807.07</c:v>
+                  <c:v>29092.72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22662.01</c:v>
+                  <c:v>27852.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23380.86</c:v>
+                  <c:v>26396.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,11 +610,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>spring</c:v>
+                  <c:v>spider-gazelle-mt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -498,32 +631,61 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X=1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X=4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X=8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X=16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X=32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X=64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$9</c:f>
+              <c:f>Sheet1!$C$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4942.68</c:v>
+                  <c:v>10960.89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9645.389999999999</c:v>
+                  <c:v>21712.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13365.49</c:v>
+                  <c:v>27886.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15394.04</c:v>
+                  <c:v>35697.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14997.89</c:v>
+                  <c:v>36744.53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15052.13</c:v>
+                  <c:v>36791.95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15667.97</c:v>
+                  <c:v>36053.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -531,15 +693,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="8"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Sheet1!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>kemal</c:v>
+                  <c:v>fasthttp-router</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -547,7 +709,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -556,32 +720,61 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X=1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X=4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X=8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X=16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X=32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X=64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$9</c:f>
+              <c:f>Sheet1!$C$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9299.01</c:v>
+                  <c:v>10626.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18025.31</c:v>
+                  <c:v>20358.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23592.16</c:v>
+                  <c:v>30474.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25750.32</c:v>
+                  <c:v>31107.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23527.11</c:v>
+                  <c:v>37379.68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22331.75</c:v>
+                  <c:v>40148.49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19368.54</c:v>
+                  <c:v>40332.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,11 +790,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2131418992"/>
-        <c:axId val="2131422576"/>
+        <c:axId val="-2141061504"/>
+        <c:axId val="-2144546944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131418992"/>
+        <c:axId val="-2141061504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131422576"/>
+        <c:crossAx val="-2144546944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -652,9 +845,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131422576"/>
+        <c:axId val="-2144546944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -672,7 +866,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -703,7 +897,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131418992"/>
+        <c:crossAx val="-2141061504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -771,7 +965,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="+mn-lt"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1344,20 +1540,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>111760</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>172720</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1638,158 +1834,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C4" s="2">
+        <v>6570.17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>11995.85</v>
+      </c>
+      <c r="E4" s="2">
+        <v>19384.64</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20083.650000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>22241.279999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>23967.68</v>
+      </c>
+      <c r="I4" s="2">
+        <v>24547.47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C5" s="2">
+        <v>11893.69</v>
+      </c>
+      <c r="D5" s="2">
+        <v>23415.25</v>
+      </c>
+      <c r="E5" s="2">
+        <v>30027.360000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>35027.75</v>
+      </c>
+      <c r="G5" s="2">
+        <v>40493.51</v>
+      </c>
+      <c r="H5" s="2">
+        <v>45090.82</v>
+      </c>
+      <c r="I5" s="2">
+        <v>48192.06</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
+      <c r="C6" s="2">
+        <v>11152.21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>19495</v>
+      </c>
+      <c r="E6" s="2">
+        <v>31390.22</v>
+      </c>
+      <c r="F6" s="2">
+        <v>29760.47</v>
+      </c>
+      <c r="G6" s="2">
+        <v>29092.720000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>27852.75</v>
+      </c>
+      <c r="I6" s="2">
+        <v>26396.7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9631.35</v>
-      </c>
-      <c r="D3" s="2">
-        <v>6324.46</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4942.68</v>
-      </c>
-      <c r="F3" s="2">
-        <v>9299.01</v>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10960.89</v>
+      </c>
+      <c r="D7" s="2">
+        <v>21712.57</v>
+      </c>
+      <c r="E7" s="2">
+        <v>27886.97</v>
+      </c>
+      <c r="F7" s="2">
+        <v>35697.339999999997</v>
+      </c>
+      <c r="G7" s="2">
+        <v>36744.53</v>
+      </c>
+      <c r="H7" s="2">
+        <v>36791.949999999997</v>
+      </c>
+      <c r="I7" s="2">
+        <v>36053.11</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>18261.419999999998</v>
-      </c>
-      <c r="D4" s="2">
-        <v>11880.28</v>
-      </c>
-      <c r="E4" s="2">
-        <v>9645.39</v>
-      </c>
-      <c r="F4" s="2">
-        <v>18025.310000000001</v>
-      </c>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10626.63</v>
+      </c>
+      <c r="D8" s="2">
+        <v>20358.05</v>
+      </c>
+      <c r="E8" s="9">
+        <v>30474.65</v>
+      </c>
+      <c r="F8" s="9">
+        <v>31107.919999999998</v>
+      </c>
+      <c r="G8" s="9">
+        <v>37379.68</v>
+      </c>
+      <c r="H8" s="9">
+        <v>40148.49</v>
+      </c>
+      <c r="I8" s="10">
+        <v>40332.019999999997</v>
+      </c>
+      <c r="J8" s="11"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>25336.34</v>
-      </c>
-      <c r="D5" s="2">
-        <v>17684.82</v>
-      </c>
-      <c r="E5" s="2">
-        <v>13365.49</v>
-      </c>
-      <c r="F5" s="2">
-        <v>23592.16</v>
-      </c>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="1">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
-        <v>25010.38</v>
-      </c>
-      <c r="D6" s="2">
-        <v>20198.53</v>
-      </c>
-      <c r="E6" s="2">
-        <v>15394.04</v>
-      </c>
-      <c r="F6" s="2">
-        <v>25750.32</v>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="1">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2">
-        <v>23253.83</v>
-      </c>
-      <c r="D7" s="2">
-        <v>21807.07</v>
-      </c>
-      <c r="E7" s="2">
-        <v>14997.89</v>
-      </c>
-      <c r="F7" s="2">
-        <v>23527.11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="1">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2">
-        <v>22220.29</v>
-      </c>
-      <c r="D8" s="2">
-        <v>22662.01</v>
-      </c>
-      <c r="E8" s="2">
-        <v>15052.13</v>
-      </c>
-      <c r="F8" s="2">
-        <v>22331.75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
-        <v>64</v>
-      </c>
-      <c r="C9" s="2">
-        <v>20957.41</v>
-      </c>
-      <c r="D9" s="2">
-        <v>23380.86</v>
-      </c>
-      <c r="E9" s="2">
-        <v>15667.97</v>
-      </c>
-      <c r="F9" s="2">
-        <v>19368.54</v>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:I2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>